<commit_message>
Apriori working fine with dataset and getting proper results
</commit_message>
<xml_diff>
--- a/Test with manipulated Dataset/ManipulatedDataset.xlsx
+++ b/Test with manipulated Dataset/ManipulatedDataset.xlsx
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N85" workbookViewId="0">
-      <selection activeCell="T113" sqref="T113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -674,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>9</v>
@@ -692,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="K4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <v>9</v>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="N4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O4">
         <v>8</v>
@@ -798,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -816,7 +816,7 @@
         <v>7</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <v>7</v>
@@ -825,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="N6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6">
         <v>8</v>
@@ -860,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -878,7 +878,7 @@
         <v>6</v>
       </c>
       <c r="K7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -887,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="N7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O7">
         <v>8</v>
@@ -922,7 +922,7 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>8</v>
@@ -984,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -1046,7 +1046,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -1064,7 +1064,7 @@
         <v>9</v>
       </c>
       <c r="K10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L10">
         <v>9</v>
@@ -1073,7 +1073,7 @@
         <v>6</v>
       </c>
       <c r="N10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O10">
         <v>7</v>
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -1126,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="K11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -1135,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="N11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O11">
         <v>8</v>
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>8</v>
@@ -1188,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="K12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L12">
         <v>8</v>
@@ -1197,7 +1197,7 @@
         <v>4</v>
       </c>
       <c r="N12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O12">
         <v>5</v>
@@ -1232,7 +1232,7 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>9</v>
@@ -1250,7 +1250,7 @@
         <v>9</v>
       </c>
       <c r="K13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L13">
         <v>9</v>
@@ -1259,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="N13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O13">
         <v>7</v>
@@ -1356,7 +1356,7 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <v>5</v>
@@ -1374,7 +1374,7 @@
         <v>9</v>
       </c>
       <c r="K15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L15">
         <v>5</v>
@@ -1383,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="N15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O15">
         <v>9</v>
@@ -1480,7 +1480,7 @@
         <v>9</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1498,7 +1498,7 @@
         <v>9</v>
       </c>
       <c r="K17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L17">
         <v>9</v>
@@ -1507,7 +1507,7 @@
         <v>8</v>
       </c>
       <c r="N17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O17">
         <v>8</v>
@@ -1542,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -1560,7 +1560,7 @@
         <v>4</v>
       </c>
       <c r="K18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L18">
         <v>4</v>
@@ -1569,7 +1569,7 @@
         <v>9</v>
       </c>
       <c r="N18">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O18">
         <v>9</v>
@@ -1666,7 +1666,7 @@
         <v>8</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -1684,7 +1684,7 @@
         <v>8</v>
       </c>
       <c r="K20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L20">
         <v>8</v>
@@ -1693,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="N20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O20">
         <v>8</v>
@@ -1790,7 +1790,7 @@
         <v>6</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>6</v>
@@ -1808,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="K22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L22">
         <v>6</v>
@@ -1817,7 +1817,7 @@
         <v>8</v>
       </c>
       <c r="N22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O22">
         <v>7</v>
@@ -1914,7 +1914,7 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -1932,7 +1932,7 @@
         <v>8</v>
       </c>
       <c r="K24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L24">
         <v>8</v>
@@ -1941,7 +1941,7 @@
         <v>4</v>
       </c>
       <c r="N24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O24">
         <v>7</v>
@@ -2224,7 +2224,7 @@
         <v>7</v>
       </c>
       <c r="E29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29">
         <v>7</v>
@@ -2242,7 +2242,7 @@
         <v>7</v>
       </c>
       <c r="K29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L29">
         <v>7</v>
@@ -2251,7 +2251,7 @@
         <v>7</v>
       </c>
       <c r="N29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O29">
         <v>8</v>
@@ -2472,7 +2472,7 @@
         <v>8</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33">
         <v>8</v>
@@ -2490,7 +2490,7 @@
         <v>8</v>
       </c>
       <c r="K33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L33">
         <v>8</v>
@@ -2499,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="N33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O33">
         <v>8</v>
@@ -2658,7 +2658,7 @@
         <v>7</v>
       </c>
       <c r="E36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F36">
         <v>7</v>
@@ -2676,7 +2676,7 @@
         <v>7</v>
       </c>
       <c r="K36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L36">
         <v>7</v>
@@ -2685,7 +2685,7 @@
         <v>6</v>
       </c>
       <c r="N36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O36">
         <v>8</v>
@@ -2720,7 +2720,7 @@
         <v>6</v>
       </c>
       <c r="E37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37">
         <v>6</v>
@@ -2738,7 +2738,7 @@
         <v>6</v>
       </c>
       <c r="K37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L37">
         <v>6</v>
@@ -2747,7 +2747,7 @@
         <v>7</v>
       </c>
       <c r="N37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O37">
         <v>8</v>
@@ -2782,7 +2782,7 @@
         <v>8</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F38">
         <v>8</v>
@@ -2800,7 +2800,7 @@
         <v>8</v>
       </c>
       <c r="K38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L38">
         <v>8</v>
@@ -2809,7 +2809,7 @@
         <v>9</v>
       </c>
       <c r="N38">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O38">
         <v>8</v>
@@ -2844,7 +2844,7 @@
         <v>10</v>
       </c>
       <c r="E39">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F39">
         <v>10</v>
@@ -2862,7 +2862,7 @@
         <v>10</v>
       </c>
       <c r="K39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L39">
         <v>10</v>
@@ -2871,7 +2871,7 @@
         <v>7</v>
       </c>
       <c r="N39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O39">
         <v>8</v>
@@ -2906,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="E40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F40">
         <v>9</v>
@@ -2924,7 +2924,7 @@
         <v>9</v>
       </c>
       <c r="K40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L40">
         <v>9</v>
@@ -2933,7 +2933,7 @@
         <v>7</v>
       </c>
       <c r="N40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O40">
         <v>8</v>
@@ -2968,7 +2968,7 @@
         <v>5</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41">
         <v>5</v>
@@ -2986,7 +2986,7 @@
         <v>5</v>
       </c>
       <c r="K41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L41">
         <v>5</v>
@@ -2995,7 +2995,7 @@
         <v>5</v>
       </c>
       <c r="N41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O41">
         <v>8</v>
@@ -3030,7 +3030,7 @@
         <v>8</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42">
         <v>8</v>
@@ -3048,7 +3048,7 @@
         <v>8</v>
       </c>
       <c r="K42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L42">
         <v>8</v>
@@ -3057,7 +3057,7 @@
         <v>8</v>
       </c>
       <c r="N42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O42">
         <v>8</v>
@@ -3092,7 +3092,7 @@
         <v>9</v>
       </c>
       <c r="E43">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F43">
         <v>9</v>
@@ -3110,7 +3110,7 @@
         <v>9</v>
       </c>
       <c r="K43">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L43">
         <v>9</v>
@@ -3119,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="N43">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O43">
         <v>6</v>
@@ -3154,7 +3154,7 @@
         <v>7</v>
       </c>
       <c r="E44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44">
         <v>7</v>
@@ -3172,7 +3172,7 @@
         <v>7</v>
       </c>
       <c r="K44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L44">
         <v>7</v>
@@ -3181,7 +3181,7 @@
         <v>6</v>
       </c>
       <c r="N44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O44">
         <v>6</v>
@@ -3216,7 +3216,7 @@
         <v>5</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45">
         <v>5</v>
@@ -3234,7 +3234,7 @@
         <v>5</v>
       </c>
       <c r="K45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L45">
         <v>5</v>
@@ -3243,7 +3243,7 @@
         <v>7</v>
       </c>
       <c r="N45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O45">
         <v>7</v>
@@ -3464,7 +3464,7 @@
         <v>7</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F49">
         <v>7</v>
@@ -3482,7 +3482,7 @@
         <v>7</v>
       </c>
       <c r="K49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L49">
         <v>7</v>
@@ -3491,7 +3491,7 @@
         <v>6</v>
       </c>
       <c r="N49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O49">
         <v>6</v>
@@ -3526,7 +3526,7 @@
         <v>8</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F50">
         <v>8</v>
@@ -3544,7 +3544,7 @@
         <v>8</v>
       </c>
       <c r="K50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L50">
         <v>8</v>
@@ -3553,7 +3553,7 @@
         <v>7</v>
       </c>
       <c r="N50">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O50">
         <v>8</v>
@@ -3650,7 +3650,7 @@
         <v>8</v>
       </c>
       <c r="E52">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F52">
         <v>8</v>
@@ -3668,7 +3668,7 @@
         <v>8</v>
       </c>
       <c r="K52">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L52">
         <v>8</v>
@@ -3677,7 +3677,7 @@
         <v>5</v>
       </c>
       <c r="N52">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O52">
         <v>7</v>
@@ -3712,7 +3712,7 @@
         <v>9</v>
       </c>
       <c r="E53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F53">
         <v>9</v>
@@ -3730,7 +3730,7 @@
         <v>9</v>
       </c>
       <c r="K53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L53">
         <v>9</v>
@@ -3739,7 +3739,7 @@
         <v>7</v>
       </c>
       <c r="N53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O53">
         <v>8</v>
@@ -3836,7 +3836,7 @@
         <v>7</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F55">
         <v>7</v>
@@ -3854,7 +3854,7 @@
         <v>7</v>
       </c>
       <c r="K55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L55">
         <v>7</v>
@@ -3863,7 +3863,7 @@
         <v>7</v>
       </c>
       <c r="N55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O55">
         <v>7</v>
@@ -3960,7 +3960,7 @@
         <v>8</v>
       </c>
       <c r="E57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F57">
         <v>8</v>
@@ -3978,7 +3978,7 @@
         <v>8</v>
       </c>
       <c r="K57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L57">
         <v>8</v>
@@ -3987,7 +3987,7 @@
         <v>8</v>
       </c>
       <c r="N57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O57">
         <v>9</v>
@@ -4022,7 +4022,7 @@
         <v>10</v>
       </c>
       <c r="E58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F58">
         <v>10</v>
@@ -4040,7 +4040,7 @@
         <v>10</v>
       </c>
       <c r="K58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L58">
         <v>10</v>
@@ -4049,7 +4049,7 @@
         <v>9</v>
       </c>
       <c r="N58">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O58">
         <v>8</v>
@@ -4084,7 +4084,7 @@
         <v>9</v>
       </c>
       <c r="E59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F59">
         <v>9</v>
@@ -4102,7 +4102,7 @@
         <v>9</v>
       </c>
       <c r="K59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L59">
         <v>9</v>
@@ -4111,7 +4111,7 @@
         <v>7</v>
       </c>
       <c r="N59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O59">
         <v>7</v>
@@ -4208,7 +4208,7 @@
         <v>8</v>
       </c>
       <c r="E61">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F61">
         <v>8</v>
@@ -4226,7 +4226,7 @@
         <v>8</v>
       </c>
       <c r="K61">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L61">
         <v>8</v>
@@ -4235,7 +4235,7 @@
         <v>6</v>
       </c>
       <c r="N61">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O61">
         <v>6</v>
@@ -4270,7 +4270,7 @@
         <v>9</v>
       </c>
       <c r="E62">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F62">
         <v>9</v>
@@ -4288,7 +4288,7 @@
         <v>9</v>
       </c>
       <c r="K62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L62">
         <v>9</v>
@@ -4332,7 +4332,7 @@
         <v>7</v>
       </c>
       <c r="E63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63">
         <v>7</v>
@@ -4350,7 +4350,7 @@
         <v>7</v>
       </c>
       <c r="K63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L63">
         <v>7</v>
@@ -4359,7 +4359,7 @@
         <v>8</v>
       </c>
       <c r="N63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O63">
         <v>8</v>
@@ -4394,7 +4394,7 @@
         <v>5</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F64">
         <v>5</v>
@@ -4412,7 +4412,7 @@
         <v>5</v>
       </c>
       <c r="K64">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L64">
         <v>5</v>
@@ -4421,7 +4421,7 @@
         <v>7</v>
       </c>
       <c r="N64">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O64">
         <v>6</v>
@@ -4518,7 +4518,7 @@
         <v>9</v>
       </c>
       <c r="E66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F66">
         <v>9</v>
@@ -4536,7 +4536,7 @@
         <v>9</v>
       </c>
       <c r="K66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L66">
         <v>9</v>
@@ -4545,7 +4545,7 @@
         <v>7</v>
       </c>
       <c r="N66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O66">
         <v>7</v>
@@ -4580,7 +4580,7 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67">
         <v>4</v>
@@ -4598,7 +4598,7 @@
         <v>4</v>
       </c>
       <c r="K67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L67">
         <v>4</v>
@@ -4607,7 +4607,7 @@
         <v>7</v>
       </c>
       <c r="N67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O67">
         <v>7</v>
@@ -4828,7 +4828,7 @@
         <v>10</v>
       </c>
       <c r="E71">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71">
         <v>10</v>
@@ -4846,7 +4846,7 @@
         <v>10</v>
       </c>
       <c r="K71">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L71">
         <v>10</v>
@@ -4855,7 +4855,7 @@
         <v>7</v>
       </c>
       <c r="N71">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O71">
         <v>7</v>
@@ -4890,7 +4890,7 @@
         <v>7</v>
       </c>
       <c r="E72">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72">
         <v>7</v>
@@ -4908,7 +4908,7 @@
         <v>7</v>
       </c>
       <c r="K72">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L72">
         <v>7</v>
@@ -4917,7 +4917,7 @@
         <v>5</v>
       </c>
       <c r="N72">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O72">
         <v>6</v>
@@ -4952,7 +4952,7 @@
         <v>6</v>
       </c>
       <c r="E73">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F73">
         <v>6</v>
@@ -4970,7 +4970,7 @@
         <v>6</v>
       </c>
       <c r="K73">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L73">
         <v>6</v>
@@ -4979,7 +4979,7 @@
         <v>4</v>
       </c>
       <c r="N73">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O73">
         <v>7</v>
@@ -5014,7 +5014,7 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F74">
         <v>8</v>
@@ -5032,7 +5032,7 @@
         <v>8</v>
       </c>
       <c r="K74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L74">
         <v>8</v>
@@ -5041,7 +5041,7 @@
         <v>5</v>
       </c>
       <c r="N74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O74">
         <v>7</v>
@@ -5076,7 +5076,7 @@
         <v>10</v>
       </c>
       <c r="E75">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F75">
         <v>10</v>
@@ -5094,7 +5094,7 @@
         <v>10</v>
       </c>
       <c r="K75">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L75">
         <v>10</v>
@@ -5103,7 +5103,7 @@
         <v>6</v>
       </c>
       <c r="N75">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O75">
         <v>7</v>
@@ -5138,7 +5138,7 @@
         <v>9</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F76">
         <v>9</v>
@@ -5156,7 +5156,7 @@
         <v>9</v>
       </c>
       <c r="K76">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L76">
         <v>9</v>
@@ -5165,7 +5165,7 @@
         <v>7</v>
       </c>
       <c r="N76">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O76">
         <v>6</v>
@@ -5200,7 +5200,7 @@
         <v>5</v>
       </c>
       <c r="E77">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F77">
         <v>5</v>
@@ -5218,7 +5218,7 @@
         <v>5</v>
       </c>
       <c r="K77">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L77">
         <v>8</v>
@@ -5227,7 +5227,7 @@
         <v>7</v>
       </c>
       <c r="N77">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O77">
         <v>6</v>
@@ -5324,7 +5324,7 @@
         <v>9</v>
       </c>
       <c r="E79">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F79">
         <v>9</v>
@@ -5342,7 +5342,7 @@
         <v>9</v>
       </c>
       <c r="K79">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L79">
         <v>9</v>
@@ -5351,7 +5351,7 @@
         <v>7</v>
       </c>
       <c r="N79">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O79">
         <v>7</v>
@@ -5448,7 +5448,7 @@
         <v>5</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F81">
         <v>5</v>
@@ -5466,7 +5466,7 @@
         <v>5</v>
       </c>
       <c r="K81">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L81">
         <v>5</v>
@@ -5475,7 +5475,7 @@
         <v>5</v>
       </c>
       <c r="N81">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O81">
         <v>5</v>
@@ -5510,7 +5510,7 @@
         <v>6</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F82">
         <v>7</v>
@@ -5528,7 +5528,7 @@
         <v>6</v>
       </c>
       <c r="K82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L82">
         <v>6</v>
@@ -5537,7 +5537,7 @@
         <v>10</v>
       </c>
       <c r="N82">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O82">
         <v>9</v>
@@ -5572,7 +5572,7 @@
         <v>9</v>
       </c>
       <c r="E83">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F83">
         <v>9</v>
@@ -5590,7 +5590,7 @@
         <v>9</v>
       </c>
       <c r="K83">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L83">
         <v>9</v>
@@ -5599,7 +5599,7 @@
         <v>8</v>
       </c>
       <c r="N83">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O83">
         <v>8</v>
@@ -5634,7 +5634,7 @@
         <v>4</v>
       </c>
       <c r="E84">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F84">
         <v>4</v>
@@ -5652,7 +5652,7 @@
         <v>4</v>
       </c>
       <c r="K84">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L84">
         <v>4</v>
@@ -5661,7 +5661,7 @@
         <v>7</v>
       </c>
       <c r="N84">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O84">
         <v>7</v>
@@ -5696,7 +5696,7 @@
         <v>5</v>
       </c>
       <c r="E85">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F85">
         <v>5</v>
@@ -5714,7 +5714,7 @@
         <v>5</v>
       </c>
       <c r="K85">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L85">
         <v>5</v>
@@ -5723,7 +5723,7 @@
         <v>7</v>
       </c>
       <c r="N85">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O85">
         <v>7</v>
@@ -5758,7 +5758,7 @@
         <v>8</v>
       </c>
       <c r="E86">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F86">
         <v>8</v>
@@ -5776,7 +5776,7 @@
         <v>8</v>
       </c>
       <c r="K86">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L86">
         <v>8</v>
@@ -5785,7 +5785,7 @@
         <v>6</v>
       </c>
       <c r="N86">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O86">
         <v>8</v>
@@ -5820,7 +5820,7 @@
         <v>9</v>
       </c>
       <c r="E87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F87">
         <v>9</v>
@@ -5838,7 +5838,7 @@
         <v>5</v>
       </c>
       <c r="K87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L87">
         <v>9</v>
@@ -5847,7 +5847,7 @@
         <v>6</v>
       </c>
       <c r="N87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O87">
         <v>7</v>
@@ -5882,7 +5882,7 @@
         <v>10</v>
       </c>
       <c r="E88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F88">
         <v>10</v>
@@ -5900,7 +5900,7 @@
         <v>10</v>
       </c>
       <c r="K88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L88">
         <v>10</v>
@@ -5909,7 +5909,7 @@
         <v>7</v>
       </c>
       <c r="N88">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O88">
         <v>7</v>
@@ -5944,7 +5944,7 @@
         <v>7</v>
       </c>
       <c r="E89">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F89">
         <v>7</v>
@@ -5962,7 +5962,7 @@
         <v>7</v>
       </c>
       <c r="K89">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L89">
         <v>7</v>
@@ -5971,7 +5971,7 @@
         <v>6</v>
       </c>
       <c r="N89">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O89">
         <v>7</v>
@@ -6006,7 +6006,7 @@
         <v>6</v>
       </c>
       <c r="E90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F90">
         <v>6</v>
@@ -6024,7 +6024,7 @@
         <v>6</v>
       </c>
       <c r="K90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L90">
         <v>6</v>
@@ -6033,7 +6033,7 @@
         <v>7</v>
       </c>
       <c r="N90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O90">
         <v>8</v>
@@ -6068,7 +6068,7 @@
         <v>8</v>
       </c>
       <c r="E91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F91">
         <v>8</v>
@@ -6086,7 +6086,7 @@
         <v>8</v>
       </c>
       <c r="K91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L91">
         <v>8</v>
@@ -6095,7 +6095,7 @@
         <v>7</v>
       </c>
       <c r="N91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O91">
         <v>7</v>
@@ -6130,7 +6130,7 @@
         <v>10</v>
       </c>
       <c r="E92">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F92">
         <v>10</v>
@@ -6254,7 +6254,7 @@
         <v>5</v>
       </c>
       <c r="E94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F94">
         <v>5</v>
@@ -6272,7 +6272,7 @@
         <v>5</v>
       </c>
       <c r="K94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L94">
         <v>5</v>
@@ -6281,7 +6281,7 @@
         <v>5</v>
       </c>
       <c r="N94">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O94">
         <v>7</v>
@@ -6316,7 +6316,7 @@
         <v>8</v>
       </c>
       <c r="E95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95">
         <v>8</v>
@@ -6334,7 +6334,7 @@
         <v>8</v>
       </c>
       <c r="K95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L95">
         <v>8</v>
@@ -6343,7 +6343,7 @@
         <v>6</v>
       </c>
       <c r="N95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O95">
         <v>7</v>
@@ -6502,7 +6502,7 @@
         <v>5</v>
       </c>
       <c r="E98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F98">
         <v>5</v>
@@ -6520,7 +6520,7 @@
         <v>5</v>
       </c>
       <c r="K98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L98">
         <v>5</v>
@@ -6529,7 +6529,7 @@
         <v>7</v>
       </c>
       <c r="N98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O98">
         <v>8</v>
@@ -6564,7 +6564,7 @@
         <v>6</v>
       </c>
       <c r="E99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F99">
         <v>6</v>
@@ -6582,7 +6582,7 @@
         <v>6</v>
       </c>
       <c r="K99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L99">
         <v>6</v>
@@ -6591,7 +6591,7 @@
         <v>7</v>
       </c>
       <c r="N99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O99">
         <v>5</v>
@@ -6626,7 +6626,7 @@
         <v>9</v>
       </c>
       <c r="E100">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F100">
         <v>9</v>
@@ -6688,7 +6688,7 @@
         <v>4</v>
       </c>
       <c r="E101">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F101">
         <v>4</v>
@@ -6706,7 +6706,7 @@
         <v>4</v>
       </c>
       <c r="K101">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L101">
         <v>4</v>
@@ -6715,7 +6715,7 @@
         <v>7</v>
       </c>
       <c r="N101">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O101">
         <v>7</v>
@@ -6750,7 +6750,7 @@
         <v>7</v>
       </c>
       <c r="E102">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F102">
         <v>7</v>
@@ -6768,7 +6768,7 @@
         <v>7</v>
       </c>
       <c r="K102">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L102">
         <v>7</v>
@@ -6777,7 +6777,7 @@
         <v>8</v>
       </c>
       <c r="N102">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O102">
         <v>8</v>
@@ -6812,7 +6812,7 @@
         <v>8</v>
       </c>
       <c r="E103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F103">
         <v>8</v>
@@ -6830,7 +6830,7 @@
         <v>8</v>
       </c>
       <c r="K103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L103">
         <v>8</v>
@@ -6839,7 +6839,7 @@
         <v>4</v>
       </c>
       <c r="N103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O103">
         <v>4</v>
@@ -6892,7 +6892,7 @@
         <v>5</v>
       </c>
       <c r="K104">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L104">
         <v>5</v>
@@ -6998,7 +6998,7 @@
         <v>4</v>
       </c>
       <c r="E106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F106">
         <v>8</v>
@@ -7016,7 +7016,7 @@
         <v>4</v>
       </c>
       <c r="K106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L106">
         <v>4</v>
@@ -7025,7 +7025,7 @@
         <v>7</v>
       </c>
       <c r="N106">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O106">
         <v>8</v>
@@ -7060,7 +7060,7 @@
         <v>8</v>
       </c>
       <c r="E107">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F107">
         <v>8</v>
@@ -7078,7 +7078,7 @@
         <v>8</v>
       </c>
       <c r="K107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L107">
         <v>7</v>
@@ -7087,7 +7087,7 @@
         <v>9</v>
       </c>
       <c r="N107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O107">
         <v>10</v>
@@ -7246,7 +7246,7 @@
         <v>4</v>
       </c>
       <c r="E110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F110">
         <v>4</v>
@@ -7264,7 +7264,7 @@
         <v>4</v>
       </c>
       <c r="K110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L110">
         <v>4</v>
@@ -7273,7 +7273,7 @@
         <v>6</v>
       </c>
       <c r="N110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O110">
         <v>8</v>
@@ -7308,7 +7308,7 @@
         <v>8</v>
       </c>
       <c r="E111">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F111">
         <v>8</v>
@@ -7326,7 +7326,7 @@
         <v>8</v>
       </c>
       <c r="K111">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L111">
         <v>8</v>
@@ -7335,7 +7335,7 @@
         <v>5</v>
       </c>
       <c r="N111">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O111">
         <v>7</v>
@@ -7432,7 +7432,7 @@
         <v>5</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F113">
         <v>5</v>
@@ -7450,7 +7450,7 @@
         <v>5</v>
       </c>
       <c r="K113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L113">
         <v>5</v>
@@ -7459,7 +7459,7 @@
         <v>8</v>
       </c>
       <c r="N113">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O113">
         <v>7</v>

</xml_diff>

<commit_message>
everything set up for final work
</commit_message>
<xml_diff>
--- a/Test with manipulated Dataset/ManipulatedDataset.xlsx
+++ b/Test with manipulated Dataset/ManipulatedDataset.xlsx
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,34 +450,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="9" width="37.6640625" customWidth="1"/>
-    <col min="10" max="10" width="28.77734375" customWidth="1"/>
-    <col min="11" max="11" width="28.88671875" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" customWidth="1"/>
-    <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="14" width="30.88671875" customWidth="1"/>
-    <col min="15" max="15" width="28.109375" customWidth="1"/>
-    <col min="16" max="16" width="19.44140625" customWidth="1"/>
-    <col min="17" max="17" width="20.21875" customWidth="1"/>
-    <col min="18" max="18" width="57.21875" customWidth="1"/>
-    <col min="19" max="19" width="32.6640625" customWidth="1"/>
-    <col min="20" max="20" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="37.799999999999997" customHeight="1">
+    <row r="1" spans="1:20" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -598,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -660,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -722,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -784,7 +783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -846,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -908,7 +907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -970,7 +969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1652,7 +1651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1776,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1900,7 +1899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2396,7 +2395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2768,7 +2767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2954,7 +2953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3574,7 +3573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3636,7 +3635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3698,7 +3697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4132,7 +4131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4194,7 +4193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4442,7 +4441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4504,7 +4503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4566,7 +4565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4628,7 +4627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4690,7 +4689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4752,7 +4751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4814,7 +4813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4876,7 +4875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5000,7 +4999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:20">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5062,7 +5061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:20">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5124,7 +5123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:20">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5186,7 +5185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:20">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5248,7 +5247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:20">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5310,7 +5309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:20">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5434,7 +5433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5496,7 +5495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5558,7 +5557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5620,7 +5619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5682,7 +5681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5744,7 +5743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5806,7 +5805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5930,7 +5929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -6054,7 +6053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -6178,7 +6177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -6240,7 +6239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -6302,7 +6301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6364,7 +6363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6426,7 +6425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:20">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6488,7 +6487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:20">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6550,7 +6549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:20">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6612,7 +6611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:20">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6674,7 +6673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:20">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6736,7 +6735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:20">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6798,7 +6797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6860,7 +6859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:20">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6984,7 +6983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:20">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -7046,7 +7045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:20">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -7108,7 +7107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:20">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -7170,7 +7169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:20">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -7232,7 +7231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:20">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -7294,7 +7293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:20">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -7356,7 +7355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:20">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -7418,7 +7417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:20">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -7491,7 +7490,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7503,7 +7502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>